<commit_message>
Evaluation v1 for current config
</commit_message>
<xml_diff>
--- a/evaluation/v1/evalute.xlsx
+++ b/evaluation/v1/evalute.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\product-kg\evaluation\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C0BD46-0646-4CF1-85BC-2FFA6D8E7436}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9865F41-29E5-4F45-9748-9F5DC419868F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9730" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9733" uniqueCount="570">
   <si>
     <t>Everyday Cheek Liptint</t>
   </si>
@@ -1791,7 +1791,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2360,7 +2390,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:E66" si="0">IF(A3=B3,"T","NA")</f>
+        <f t="shared" ref="C3:C66" si="0">IF(A3=B3,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D3" t="s">
@@ -3576,7 +3606,7 @@
         <v>7</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:E130" si="2">IF(A67=B67,"T","NA")</f>
+        <f t="shared" ref="C67:C130" si="2">IF(A67=B67,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D67" t="s">
@@ -4792,7 +4822,7 @@
         <v>39</v>
       </c>
       <c r="C131" t="str">
-        <f t="shared" ref="C131:E194" si="4">IF(A131=B131,"T","NA")</f>
+        <f t="shared" ref="C131:C194" si="4">IF(A131=B131,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D131" t="s">
@@ -6008,7 +6038,7 @@
         <v>1</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" ref="C195:E258" si="6">IF(A195=B195,"T","NA")</f>
+        <f t="shared" ref="C195:C258" si="6">IF(A195=B195,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D195" t="s">
@@ -7224,7 +7254,7 @@
         <v>41</v>
       </c>
       <c r="C259" t="str">
-        <f t="shared" ref="C259:E322" si="8">IF(A259=B259,"T","NA")</f>
+        <f t="shared" ref="C259:C322" si="8">IF(A259=B259,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D259" t="s">
@@ -8434,7 +8464,7 @@
         <v>89</v>
       </c>
       <c r="C323" t="str">
-        <f t="shared" ref="C323:E386" si="10">IF(A323=B323,"T","NA")</f>
+        <f t="shared" ref="C323:C386" si="10">IF(A323=B323,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D323" t="s">
@@ -9650,7 +9680,7 @@
         <v>1</v>
       </c>
       <c r="C387" t="str">
-        <f t="shared" ref="C387:E450" si="12">IF(A387=B387,"T","NA")</f>
+        <f t="shared" ref="C387:C450" si="12">IF(A387=B387,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D387" t="s">
@@ -10866,7 +10896,7 @@
         <v>85</v>
       </c>
       <c r="C451" t="str">
-        <f t="shared" ref="C451:E514" si="14">IF(A451=B451,"T","NA")</f>
+        <f t="shared" ref="C451:C514" si="14">IF(A451=B451,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D451" t="s">
@@ -12082,7 +12112,7 @@
         <v>1</v>
       </c>
       <c r="C515" t="str">
-        <f t="shared" ref="C515:E578" si="16">IF(A515=B515,"T","NA")</f>
+        <f t="shared" ref="C515:C578" si="16">IF(A515=B515,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D515" t="s">
@@ -13298,7 +13328,7 @@
         <v>1</v>
       </c>
       <c r="C579" t="str">
-        <f t="shared" ref="C579:E642" si="18">IF(A579=B579,"T","NA")</f>
+        <f t="shared" ref="C579:C642" si="18">IF(A579=B579,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D579" t="s">
@@ -14514,7 +14544,7 @@
         <v>1</v>
       </c>
       <c r="C643" t="str">
-        <f t="shared" ref="C643:E706" si="20">IF(A643=B643,"T","NA")</f>
+        <f t="shared" ref="C643:C706" si="20">IF(A643=B643,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D643" t="s">
@@ -15730,7 +15760,7 @@
         <v>3</v>
       </c>
       <c r="C707" t="str">
-        <f t="shared" ref="C707:E770" si="22">IF(A707=B707,"T","NA")</f>
+        <f t="shared" ref="C707:C770" si="22">IF(A707=B707,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D707" t="s">
@@ -16946,7 +16976,7 @@
         <v>213</v>
       </c>
       <c r="C771" t="str">
-        <f t="shared" ref="C771:E834" si="24">IF(A771=B771,"T","NA")</f>
+        <f t="shared" ref="C771:C834" si="24">IF(A771=B771,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D771" t="s">
@@ -18162,7 +18192,7 @@
         <v>246</v>
       </c>
       <c r="C835" t="str">
-        <f t="shared" ref="C835:E898" si="26">IF(A835=B835,"T","NA")</f>
+        <f t="shared" ref="C835:C898" si="26">IF(A835=B835,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D835" t="s">
@@ -19378,7 +19408,7 @@
         <v>282</v>
       </c>
       <c r="C899" t="str">
-        <f t="shared" ref="C899:E962" si="28">IF(A899=B899,"T","NA")</f>
+        <f t="shared" ref="C899:C962" si="28">IF(A899=B899,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D899" t="s">
@@ -20594,7 +20624,7 @@
         <v>312</v>
       </c>
       <c r="C963" t="str">
-        <f t="shared" ref="C963:E1026" si="30">IF(A963=B963,"T","NA")</f>
+        <f t="shared" ref="C963:C1026" si="30">IF(A963=B963,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D963" t="s">
@@ -21810,7 +21840,7 @@
         <v>342</v>
       </c>
       <c r="C1027" t="str">
-        <f t="shared" ref="C1027:E1090" si="32">IF(A1027=B1027,"T","NA")</f>
+        <f t="shared" ref="C1027:C1090" si="32">IF(A1027=B1027,"T","NA")</f>
         <v>NA</v>
       </c>
       <c r="D1027" t="s">
@@ -23026,7 +23056,7 @@
         <v>333</v>
       </c>
       <c r="C1091" t="str">
-        <f t="shared" ref="C1091:E1154" si="34">IF(A1091=B1091,"T","NA")</f>
+        <f t="shared" ref="C1091:C1154" si="34">IF(A1091=B1091,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D1091" t="s">
@@ -24242,7 +24272,7 @@
         <v>377</v>
       </c>
       <c r="C1155" t="str">
-        <f t="shared" ref="C1155:E1218" si="36">IF(A1155=B1155,"T","NA")</f>
+        <f t="shared" ref="C1155:C1218" si="36">IF(A1155=B1155,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D1155" t="s">
@@ -25458,7 +25488,7 @@
         <v>389</v>
       </c>
       <c r="C1219" t="str">
-        <f t="shared" ref="C1219:E1282" si="38">IF(A1219=B1219,"T","NA")</f>
+        <f t="shared" ref="C1219:C1282" si="38">IF(A1219=B1219,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D1219" t="s">
@@ -26653,7 +26683,7 @@
         <v>405</v>
       </c>
       <c r="C1283" t="str">
-        <f t="shared" ref="C1283:E1346" si="40">IF(A1283=B1283,"T","NA")</f>
+        <f t="shared" ref="C1283:C1346" si="40">IF(A1283=B1283,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="E1283" t="str">
@@ -27818,7 +27848,7 @@
         <v>234</v>
       </c>
       <c r="C1347" t="str">
-        <f t="shared" ref="C1347:E1410" si="42">IF(A1347=B1347,"T","NA")</f>
+        <f t="shared" ref="C1347:C1410" si="42">IF(A1347=B1347,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D1347" t="s">
@@ -28986,7 +29016,7 @@
         <v>418</v>
       </c>
       <c r="C1411" t="str">
-        <f t="shared" ref="C1411:E1474" si="44">IF(A1411=B1411,"T","NA")</f>
+        <f t="shared" ref="C1411:C1474" si="44">IF(A1411=B1411,"T","NA")</f>
         <v>NA</v>
       </c>
       <c r="D1411" t="s">
@@ -30202,7 +30232,7 @@
         <v>85</v>
       </c>
       <c r="C1475" t="str">
-        <f t="shared" ref="C1475:E1538" si="46">IF(A1475=B1475,"T","NA")</f>
+        <f t="shared" ref="C1475:C1538" si="46">IF(A1475=B1475,"T","NA")</f>
         <v>T</v>
       </c>
       <c r="D1475" t="s">
@@ -31373,7 +31403,7 @@
         <v>465</v>
       </c>
       <c r="C1539" t="str">
-        <f t="shared" ref="C1539:E1602" si="48">IF(A1539=B1539,"T","NA")</f>
+        <f t="shared" ref="C1539:C1602" si="48">IF(A1539=B1539,"T","NA")</f>
         <v>NA</v>
       </c>
       <c r="D1539" t="s">
@@ -32397,7 +32427,7 @@
         <v>529</v>
       </c>
       <c r="C1603" t="str">
-        <f t="shared" ref="C1603:E1637" si="50">IF(A1603=B1603,"T","NA")</f>
+        <f t="shared" ref="C1603:C1637" si="50">IF(A1603=B1603,"T","NA")</f>
         <v>NA</v>
       </c>
       <c r="D1603" t="s">
@@ -32954,24 +32984,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32982,10 +33012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6EECF-5F2E-40E0-9136-9EC9B8C8ED00}">
-  <dimension ref="A1:G1640"/>
+  <dimension ref="A1:G1641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1503" workbookViewId="0">
-      <selection activeCell="B1514" sqref="B1514"/>
+    <sheetView tabSelected="1" topLeftCell="A627" workbookViewId="0">
+      <selection activeCell="E627" sqref="E627"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34266,7 +34296,7 @@
         <v>4</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" ref="E67:E130" si="3">IF(B68=D68,"T","NA")</f>
+        <f t="shared" ref="E68:E130" si="3">IF(B68=D68,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -36649,7 +36679,7 @@
         <v>1</v>
       </c>
       <c r="E195" t="str">
-        <f t="shared" ref="E195:E258" si="7">IF(B195=D195,"T","NA")</f>
+        <f t="shared" ref="E195:E257" si="7">IF(B195=D195,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -44801,14 +44831,13 @@
         <v>166</v>
       </c>
       <c r="C627" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D627" t="s">
         <v>166</v>
       </c>
-      <c r="E627" t="str">
-        <f t="shared" si="19"/>
-        <v>T</v>
+      <c r="E627" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.3">
@@ -45199,14 +45228,13 @@
         <v>166</v>
       </c>
       <c r="C648" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D648" t="s">
         <v>166</v>
       </c>
-      <c r="E648" t="str">
-        <f t="shared" si="21"/>
-        <v>T</v>
+      <c r="E648" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.3">
@@ -46158,14 +46186,13 @@
         <v>166</v>
       </c>
       <c r="C699" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D699" t="s">
         <v>166</v>
       </c>
-      <c r="E699" t="str">
-        <f t="shared" si="21"/>
-        <v>T</v>
+      <c r="E699" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.3">
@@ -53606,7 +53633,7 @@
         <v>312</v>
       </c>
       <c r="E1093" t="str">
-        <f t="shared" ref="E1091:E1154" si="35">IF(B1093=D1093,"T","NA")</f>
+        <f t="shared" ref="E1093:E1154" si="35">IF(B1093=D1093,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -61621,29 +61648,29 @@
     <row r="1525" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C1525">
         <f>COUNTIF(C2:C1524,"T")</f>
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="E1525">
         <f>COUNTIF(E2:E1524,"T")</f>
-        <v>1430</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1526" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1526">
         <f>C1525/(C1525+C1526)*100</f>
-        <v>99.934253780407616</v>
+        <v>99.737015121630506</v>
       </c>
       <c r="C1526">
         <f>COUNTIF(C2:C1524,"F")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1526">
         <f>E1525/(E1525+E1526)*100</f>
-        <v>96.686950642325897</v>
+        <v>96.4841108857336</v>
       </c>
       <c r="E1526">
         <f>COUNTIF(E2:E1524,"F")</f>
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="1527" spans="1:5" x14ac:dyDescent="0.3">
@@ -63450,48 +63477,73 @@
         <v>90.265486725663706</v>
       </c>
     </row>
+    <row r="1641" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E1641">
+        <f>COUNTIF(E2:E1639,"T")</f>
+        <v>1529</v>
+      </c>
+      <c r="F1641">
+        <f>COUNTIF(E2:E1639,"F")</f>
+        <v>63</v>
+      </c>
+      <c r="G1641">
+        <f>E1641/(E1641+F1641) *100</f>
+        <v>96.042713567839201</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1639">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1524 E1527:E1640">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1640">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1525:E1526">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1641:F1641">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Init improvement, found out getting worse
</commit_message>
<xml_diff>
--- a/evaluation/v1/evalute.xlsx
+++ b/evaluation/v1/evalute.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\product-kg\evaluation\v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\product-kg\evaluation\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A7CBF2-848A-4BA4-AC25-232873C8EF8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE5142-0D4E-4336-8995-E4E2C3FBF27F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1804,21 +1804,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2208,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1640"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1639" workbookViewId="0">
-      <selection activeCell="E269" sqref="E269"/>
+    <sheetView tabSelected="1" topLeftCell="A1563" workbookViewId="0">
+      <selection activeCell="E1531" sqref="E1531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3491,7 +3491,7 @@
         <v>4</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" ref="E67:E130" si="3">IF(B68=D68,"T","NA")</f>
+        <f t="shared" ref="E68:E130" si="3">IF(B68=D68,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -5874,7 +5874,7 @@
         <v>1</v>
       </c>
       <c r="E195" t="str">
-        <f t="shared" ref="E195:E258" si="7">IF(B195=D195,"T","NA")</f>
+        <f t="shared" ref="E195:E257" si="7">IF(B195=D195,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -21592,7 +21592,7 @@
         <v>342</v>
       </c>
       <c r="E1027" t="str">
-        <f t="shared" ref="E1027:E1090" si="32">IF(B1027=D1027,"T","NA")</f>
+        <f t="shared" ref="E1027:E1089" si="32">IF(B1027=D1027,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -22813,7 +22813,7 @@
         <v>312</v>
       </c>
       <c r="E1092" t="str">
-        <f t="shared" ref="E1091:E1154" si="35">IF(B1092=D1092,"T","NA")</f>
+        <f t="shared" ref="E1092:E1154" si="35">IF(B1092=D1092,"T","NA")</f>
         <v>T</v>
       </c>
     </row>
@@ -30914,7 +30914,7 @@
         <v>454</v>
       </c>
       <c r="E1530" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1531" spans="1:5" x14ac:dyDescent="0.3">
@@ -32632,17 +32632,17 @@
     <row r="1639" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E1639">
         <f>COUNTIF(E1526:E1638,"T")</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F1639">
         <f>COUNTIF(E1526:E1638,"F")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1640" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E1640">
         <f>E1639/(E1639+F1639)*100</f>
-        <v>90.265486725663706</v>
+        <v>89.380530973451329</v>
       </c>
     </row>
   </sheetData>
@@ -32670,18 +32670,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1522 E1526:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1523:E1525">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>